<commit_message>
Mudança de variáveis e adicionado relatorio
Mudei o nome de algumas variáveis, corrigi alguns erros básicos e adicionei a função de relatório.
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Professores" sheetId="1" r:id="rId1"/>
@@ -40,13 +40,13 @@
     <t>Codigo da Disciplina</t>
   </si>
   <si>
+    <t>Nota 1</t>
+  </si>
+  <si>
+    <t>Nota 2</t>
+  </si>
+  <si>
     <t>Matricula do Aluno</t>
-  </si>
-  <si>
-    <t>Nota 1</t>
-  </si>
-  <si>
-    <t>Nota 2</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +467,7 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,16 +505,17 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>